<commit_message>
antes de optimizar todo el código
</commit_message>
<xml_diff>
--- a/Basededatos/FURANOS.xlsx
+++ b/Basededatos/FURANOS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roquispec\OneDrive - LUZ DEL SUR S.A.A\Documentos\Estudios de Ingreso\ProyectoRyD_V2\Basededatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luzdelsurlds-my.sharepoint.com/personal/roquispec_luzdelsur_com_pe/Documents/Documentos/Estudios de Ingreso/ProyectoRyD_V2/Basededatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{493C8160-5064-44A0-A47F-7B162137B826}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF41E667-FB2B-4005-BB4A-618141E06FE7}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="113_{52009395-6EC5-4C11-AAE0-9356E77AADA1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F8AFC9F-2A25-44BE-B09B-11EFE2C1EEB4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{71916C58-564B-4457-BF76-DAA941C95708}"/>
   </bookViews>
@@ -20,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
     </ext>
@@ -37,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>SERIE</t>
   </si>
@@ -364,6 +355,12 @@
   </si>
   <si>
     <t>750005-01</t>
+  </si>
+  <si>
+    <t>TempR</t>
+  </si>
+  <si>
+    <t>HumR</t>
   </si>
 </sst>
 </file>
@@ -406,7 +403,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -429,11 +426,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -444,6 +450,9 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,10 +771,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B9FE8D7-0ED1-4C7D-B4DF-32AEE144EFAC}">
-  <dimension ref="B2:D135"/>
+  <dimension ref="B2:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="D143" sqref="D143"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +785,7 @@
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -786,8 +795,14 @@
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
@@ -798,7 +813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -809,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -820,7 +835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -831,7 +846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>551873</v>
       </c>
@@ -842,7 +857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>551875</v>
       </c>
@@ -853,7 +868,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>551874</v>
       </c>
@@ -864,7 +879,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -875,7 +890,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -886,7 +901,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
@@ -897,7 +912,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
@@ -908,7 +923,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
@@ -919,7 +934,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>13</v>
       </c>
@@ -930,7 +945,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="4">
         <v>185634</v>
       </c>

</xml_diff>